<commit_message>
Update the test files to include distributed alignments.
Both in horizontal and vertical directions.
</commit_message>
<xml_diff>
--- a/test/xlsx/text-alignment/input.xlsx
+++ b/test/xlsx/text-alignment/input.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
   <si>
     <t>Text</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Horizontal justification looks like this.</t>
+  </si>
+  <si>
+    <t>Distributed</t>
+  </si>
+  <si>
+    <t>Both horizontally and vertically distributed.</t>
   </si>
 </sst>
 </file>
@@ -118,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -197,6 +203,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="distributed" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -236,8 +245,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18669C66-4DC2-47E8-9FEB-658A3A486B2C}" name="Table1" displayName="Table1" ref="A1:C27" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C27" xr:uid="{D7EA29C0-BEE8-40FC-883C-1E11F1ADEF91}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18669C66-4DC2-47E8-9FEB-658A3A486B2C}" name="Table1" displayName="Table1" ref="A1:C28" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C28" xr:uid="{D7EA29C0-BEE8-40FC-883C-1E11F1ADEF91}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CBA1246F-C525-44D4-88D0-83C065CB6EE1}" name="Horizontal"/>
     <tableColumn id="2" xr3:uid="{3927AC1B-EF3A-4AD1-8F5C-73F068C53B96}" name="Vertical"/>
@@ -544,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C838077F-EB12-4D1F-88F1-3327DA77722A}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,6 +863,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="28" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>